<commit_message>
Added a coffee edible portions value to the IMPACT V19 xlsx file. Lots of changes to nutModSpiderGraph Added error checking in nutrientModFunctions shifted a column to the right (replacing a blank column) in DRI_IOM_V7.xlsx
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/DRI_IOM_V7.xlsx
+++ b/data-raw/NutrientData/DRI_IOM_V7.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27217"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="900" windowWidth="22640" windowHeight="14600" activeTab="6"/>
+    <workbookView xWindow="1220" yWindow="900" windowWidth="22640" windowHeight="14600" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="10" r:id="rId1"/>
@@ -943,7 +943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18:H23"/>
     </sheetView>
   </sheetViews>
@@ -3969,7 +3969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
@@ -6651,15 +6651,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="1"/>
+    <col min="3" max="8" width="8.83203125" style="1"/>
+    <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.2">
@@ -6684,8 +6685,7 @@
       <c r="G1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>52</v>
       </c>
       <c r="J1" s="2"/>
@@ -6712,7 +6712,7 @@
       <c r="G2" s="1">
         <v>60</v>
       </c>
-      <c r="I2" s="18">
+      <c r="H2" s="18">
         <v>9.1</v>
       </c>
       <c r="K2" s="2"/>
@@ -6742,7 +6742,7 @@
       <c r="G3" s="1">
         <v>95</v>
       </c>
-      <c r="I3" s="18">
+      <c r="H3" s="18">
         <v>11</v>
       </c>
       <c r="K3" s="2"/>
@@ -6766,8 +6766,7 @@
       <c r="G4" s="6">
         <v>65</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2">
+      <c r="H4" s="2">
         <v>20</v>
       </c>
       <c r="J4" s="2"/>
@@ -6798,8 +6797,7 @@
       <c r="G5" s="6">
         <v>65</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2">
+      <c r="H5" s="2">
         <v>30</v>
       </c>
       <c r="J5" s="2"/>
@@ -6830,8 +6828,7 @@
       <c r="G6" s="6">
         <v>65</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2">
+      <c r="H6" s="2">
         <v>30</v>
       </c>
       <c r="J6" s="2"/>
@@ -6862,8 +6859,7 @@
       <c r="G7" s="6">
         <v>65</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2">
+      <c r="H7" s="2">
         <v>30</v>
       </c>
       <c r="J7" s="2"/>
@@ -6892,8 +6888,7 @@
       <c r="G8" s="6">
         <v>65</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2">
+      <c r="H8" s="2">
         <v>35</v>
       </c>
       <c r="J8" s="2"/>
@@ -6922,8 +6917,7 @@
       <c r="G9" s="6">
         <v>65</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2">
+      <c r="H9" s="2">
         <v>35</v>
       </c>
       <c r="J9" s="2"/>
@@ -6952,8 +6946,7 @@
       <c r="G10" s="6">
         <v>65</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2">
+      <c r="H10" s="2">
         <v>35</v>
       </c>
       <c r="J10" s="2"/>
@@ -6982,8 +6975,7 @@
       <c r="G11" s="6">
         <v>65</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2">
+      <c r="H11" s="2">
         <v>35</v>
       </c>
       <c r="J11" s="2"/>
@@ -7014,8 +7006,7 @@
       <c r="G12" s="6">
         <v>65</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2">
+      <c r="H12" s="2">
         <v>30</v>
       </c>
       <c r="J12" s="2"/>
@@ -7044,8 +7035,7 @@
       <c r="G13" s="6">
         <v>65</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2">
+      <c r="H13" s="2">
         <v>30</v>
       </c>
       <c r="J13" s="2"/>
@@ -7074,8 +7064,7 @@
       <c r="G14" s="6">
         <v>65</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2">
+      <c r="H14" s="2">
         <v>35</v>
       </c>
       <c r="J14" s="2"/>
@@ -7104,8 +7093,7 @@
       <c r="G15" s="6">
         <v>65</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2">
+      <c r="H15" s="2">
         <v>35</v>
       </c>
       <c r="J15" s="2"/>
@@ -7134,8 +7122,7 @@
       <c r="G16" s="6">
         <v>65</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2">
+      <c r="H16" s="2">
         <v>35</v>
       </c>
       <c r="J16" s="2"/>
@@ -7164,8 +7151,7 @@
       <c r="G17" s="6">
         <v>65</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2">
+      <c r="H17" s="2">
         <v>35</v>
       </c>
       <c r="J17" s="2"/>
@@ -7194,8 +7180,7 @@
       <c r="G18" s="6">
         <v>65</v>
       </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2">
+      <c r="H18" s="2">
         <v>35</v>
       </c>
       <c r="J18" s="2"/>
@@ -7224,8 +7209,7 @@
       <c r="G19" s="6">
         <v>65</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2">
+      <c r="H19" s="2">
         <v>35</v>
       </c>
       <c r="J19" s="2"/>
@@ -7254,8 +7238,7 @@
       <c r="G20" s="6">
         <v>65</v>
       </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2">
+      <c r="H20" s="2">
         <v>35</v>
       </c>
       <c r="J20" s="2"/>
@@ -7284,8 +7267,7 @@
       <c r="G21" s="6">
         <v>65</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2">
+      <c r="H21" s="2">
         <v>35</v>
       </c>
       <c r="J21" s="2"/>
@@ -7314,8 +7296,7 @@
       <c r="G22" s="6">
         <v>65</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2">
+      <c r="H22" s="2">
         <v>35</v>
       </c>
     </row>
@@ -7339,8 +7320,7 @@
       <c r="G23" s="6">
         <v>65</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2">
+      <c r="H23" s="2">
         <v>35</v>
       </c>
     </row>

</xml_diff>